<commit_message>
update ordering sheet and add stl files
</commit_message>
<xml_diff>
--- a/ordering_sheet.xlsx
+++ b/ordering_sheet.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\workspace\mece4611\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7962868-3893-4EED-BB7A-C5A9334AE014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C27447A-EEED-4423-A2DA-8692E25EF943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11850" yWindow="5205" windowWidth="28800" windowHeight="15435" xr2:uid="{346330F8-C7D1-4ADB-8934-51C1B9D10A59}"/>
+    <workbookView xWindow="5550" yWindow="4170" windowWidth="21600" windowHeight="11325" xr2:uid="{346330F8-C7D1-4ADB-8934-51C1B9D10A59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>item</t>
   </si>
@@ -61,19 +59,64 @@
   </si>
   <si>
     <t>0.375x1.25" extension spring with hook ends</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/9271K403/</t>
+  </si>
+  <si>
+    <t>1.25" leg, 0.4" OD, 0.25" ID_Torsion Spring</t>
+  </si>
+  <si>
+    <t>1/4" Shoulder Diameter, 2-1/2" Shoulder Length, 10-24 Thread, shoulder screw</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/91259A105/</t>
+  </si>
+  <si>
+    <t>8-32, 3/4" Long button head screw</t>
+  </si>
+  <si>
+    <t>8-32, 2" Long button head screw</t>
+  </si>
+  <si>
+    <t>8-32 thin nylock nuts</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92949A197/</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/90633A009/</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/92949A207/</t>
+  </si>
+  <si>
+    <t>total:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF336633"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -96,8 +139,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{777AF586-F061-44AE-9670-FF63D9F74B4E}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,7 +473,7 @@
     <col min="5" max="5" width="40.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -442,8 +489,15 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1">
+        <f>SUM(C2:C19)</f>
+        <v>34.270000000000003</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -461,7 +515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -479,61 +533,121 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5.38</v>
+      </c>
       <c r="D4">
         <f t="shared" si="0"/>
+        <v>10.76</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>2.42</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>9.68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>6.53</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>6.53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>5.77</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>5.77</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>3.23</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>3.23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D6">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D7">
-        <f t="shared" si="0"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <f>B12*C12</f>
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D10">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D11">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -541,5 +655,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>